<commit_message>
Added modified old Li200R Base
</commit_message>
<xml_diff>
--- a/Hardware Information/Calibration Constants.xlsx
+++ b/Hardware Information/Calibration Constants.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Constants</t>
   </si>
@@ -111,17 +111,79 @@
   </si>
   <si>
     <t>LEMS Serial Number</t>
+  </si>
+  <si>
+    <t>36.5KXBK-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/yageo/MFR-25FBF52-36K5/36.5KXBK-ND/13325</t>
+  </si>
+  <si>
+    <t>37.4KXBK-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/yageo/MFR-25FBF52-37K4/37.4KXBK-ND/13327</t>
+  </si>
+  <si>
+    <t>39.2KXBK-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/yageo/MFR-25FBF52-39K2/39.2KXBK-ND/13331</t>
+  </si>
+  <si>
+    <t>33.2KXBK-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/yageo/MFR-25FBF52-33K2/33.2KXBK-ND/13317</t>
+  </si>
+  <si>
+    <t>57.6KXBK-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/yageo/MFR-25FBF52-57K6/57.6KXBK-ND/13426</t>
+  </si>
+  <si>
+    <t>S62KCACT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNMF14FTC62K0/S62KCACT-ND/2617523</t>
+  </si>
+  <si>
+    <t>59.0KXBK-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/yageo/MFR-25FBF52-59K/59.0KXBK-ND/13428</t>
+  </si>
+  <si>
+    <t>64.9KXBK-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/yageo/MFR-25FBF52-64K9/64.9KXBK-ND/13436</t>
+  </si>
+  <si>
+    <t>56.2KXBK-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/yageo/MFR-25FBF52-56K2/56.2KXBK-ND/13424</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0000E+00"/>
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,22 +217,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,7 +531,8 @@
     <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -496,7 +563,7 @@
       <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -528,6 +595,22 @@
         <f>(F2*$B$2)*G2</f>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I2">
+        <v>36500</v>
+      </c>
+      <c r="J2">
+        <f>(F2*$B$2)*I2</f>
+        <v>4.0532520000000005</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -554,6 +637,22 @@
         <f t="shared" ref="H3:H13" si="1">(F3*$B$2)*G3</f>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I3">
+        <v>37400</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J13" si="2">(F3*$B$2)*I3</f>
+        <v>4.0423416000000003</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -580,6 +679,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I4">
+        <v>39200</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>4.0482624000000005</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
@@ -597,6 +712,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I5">
+        <v>33200</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>4.0736400000000001</v>
+      </c>
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
@@ -614,6 +745,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I6">
+        <v>57600</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>4.0296960000000004</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
@@ -631,6 +778,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I7">
+        <v>62000</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>4.086792</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
@@ -648,6 +811,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I8">
+        <v>59000</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>4.036308</v>
+      </c>
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
@@ -665,6 +844,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I9">
+        <v>59000</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>4.0278119999999999</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
@@ -682,6 +877,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I10">
+        <v>59000</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>4.0476359999999998</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
@@ -699,6 +910,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I11">
+        <v>64900</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>4.0949304</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
@@ -716,6 +943,22 @@
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
       </c>
+      <c r="I12">
+        <v>59000</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>4.0922400000000003</v>
+      </c>
+      <c r="K12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
@@ -732,6 +975,22 @@
       <c r="H13">
         <f t="shared" si="1"/>
         <v>4.0960000000000001</v>
+      </c>
+      <c r="I13">
+        <v>56200</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>4.0430280000000005</v>
+      </c>
+      <c r="K13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>